<commit_message>
updated figures for part I
</commit_message>
<xml_diff>
--- a/CSVs/TableS1.xlsx
+++ b/CSVs/TableS1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>count</t>
   </si>
@@ -22,52 +22,85 @@
     <t>gender</t>
   </si>
   <si>
+    <t>age_bin</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>typical_sleep_bin</t>
+  </si>
+  <si>
     <t>anxiety</t>
   </si>
   <si>
-    <t>education</t>
+    <t>prev_night_sleep_bin</t>
   </si>
   <si>
     <t>depression</t>
   </si>
   <si>
+    <t>Female</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
+    <t>Bachelor's Degree</t>
+  </si>
+  <si>
     <t>High School Diploma</t>
   </si>
   <si>
     <t>Master's Degree</t>
   </si>
   <si>
-    <t>Bachelor's Degree</t>
-  </si>
-  <si>
     <t>Doctoral or Professional Degree</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
+    <t>Not during the past month</t>
+  </si>
+  <si>
     <t>Less than once a week</t>
   </si>
   <si>
     <t>Once or twice a week</t>
   </si>
   <si>
-    <t>Not during the past month</t>
+    <t>Three or more times a week</t>
   </si>
   <si>
     <t>Every day</t>
   </si>
   <si>
-    <t>Three or more times a week</t>
+    <t>18-30</t>
+  </si>
+  <si>
+    <t>30-40</t>
+  </si>
+  <si>
+    <t>40-50</t>
+  </si>
+  <si>
+    <t>50-60</t>
+  </si>
+  <si>
+    <t>60+</t>
+  </si>
+  <si>
+    <t>0-6</t>
+  </si>
+  <si>
+    <t>6-8</t>
+  </si>
+  <si>
+    <t>8+</t>
   </si>
 </sst>
 </file>
@@ -425,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,7 +474,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>6797</v>
@@ -450,7 +483,7 @@
     <row r="3" spans="1:3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>4013</v>
@@ -459,7 +492,7 @@
     <row r="4" spans="1:3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>76</v>
@@ -470,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>4532</v>
@@ -479,7 +512,7 @@
     <row r="6" spans="1:3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>2599</v>
@@ -488,7 +521,7 @@
     <row r="7" spans="1:3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>2368</v>
@@ -497,7 +530,7 @@
     <row r="8" spans="1:3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>1148</v>
@@ -506,7 +539,7 @@
     <row r="9" spans="1:3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>239</v>
@@ -514,10 +547,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>4116</v>
@@ -526,7 +559,7 @@
     <row r="11" spans="1:3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>2589</v>
@@ -535,7 +568,7 @@
     <row r="12" spans="1:3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>1882</v>
@@ -544,7 +577,7 @@
     <row r="13" spans="1:3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <v>1271</v>
@@ -553,7 +586,7 @@
     <row r="14" spans="1:3">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>1028</v>
@@ -561,10 +594,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>4702</v>
@@ -573,7 +606,7 @@
     <row r="16" spans="1:3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>2814</v>
@@ -582,7 +615,7 @@
     <row r="17" spans="1:3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>1762</v>
@@ -591,7 +624,7 @@
     <row r="18" spans="1:3">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>957</v>
@@ -600,17 +633,125 @@
     <row r="19" spans="1:3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>651</v>
       </c>
     </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>2911</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>2688</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>2154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>5315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>5102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>5527</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>3205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>2154</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A28:A30"/>
     <mergeCell ref="A15:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>